<commit_message>
Changed stock of all commodities
Former-commit-id: 3526b281a23de5fdac22256ad5d1e2d282d8ba5e [formerly ca30a4fbc61b8d7a3af0e488fccb7bc76dd53fdf]
Former-commit-id: 251b5affb263a09e08d6c78d56aa2f7d5c314740
</commit_message>
<xml_diff>
--- a/input1.xlsx
+++ b/input1.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arfc\Documents\GitHub\i2cner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7C852B55-90E8-453A-B56B-B4857D255E2E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7EBE938-AC5C-44C0-9176-89E6E7EE652B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7545" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="CO2" sheetId="3" r:id="rId3"/>
+    <sheet name="DMD and STOCK" sheetId="1" r:id="rId1"/>
+    <sheet name="LCoE" sheetId="4" r:id="rId2"/>
+    <sheet name="CO2 coeff" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="179017" fullCalcOnLoad="1"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="55">
   <si>
     <t>CAP2ACT</t>
   </si>
@@ -187,18 +188,12 @@
   </si>
   <si>
     <t>OLD</t>
-  </si>
-  <si>
-    <t>Nuclear Stock</t>
-  </si>
-  <si>
-    <t>Nuc Cap</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; &quot;"/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00;[Red]&quot;-&quot;[$$-409]#,##0.00"/>
@@ -325,7 +320,7 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -333,33 +328,34 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="25">
-    <cellStyle name="20% - Accent5 2" xfId="6"/>
-    <cellStyle name="Comma 2" xfId="7"/>
-    <cellStyle name="Excel_BuiltIn_20% - Accent5 1" xfId="8"/>
-    <cellStyle name="Heading" xfId="1"/>
-    <cellStyle name="Heading1" xfId="2"/>
+    <cellStyle name="20% - Accent5 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Comma 2" xfId="7" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Excel_BuiltIn_20% - Accent5 1" xfId="8" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Heading" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Heading1" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Normal 10" xfId="9"/>
-    <cellStyle name="Normal 2" xfId="10"/>
-    <cellStyle name="Normal 3" xfId="11"/>
-    <cellStyle name="Normal 4" xfId="12"/>
-    <cellStyle name="Normal 4 2" xfId="13"/>
-    <cellStyle name="Normal 5" xfId="14"/>
-    <cellStyle name="Normal 6" xfId="15"/>
-    <cellStyle name="Normal 7" xfId="16"/>
-    <cellStyle name="Normal 8" xfId="17"/>
-    <cellStyle name="Normal 9" xfId="5"/>
-    <cellStyle name="Normal 9 2" xfId="18"/>
-    <cellStyle name="Normale_B2020" xfId="19"/>
-    <cellStyle name="Percent 2" xfId="21"/>
-    <cellStyle name="Percent 3" xfId="22"/>
-    <cellStyle name="Percent 4" xfId="23"/>
-    <cellStyle name="Percent 5" xfId="20"/>
-    <cellStyle name="Result" xfId="3"/>
-    <cellStyle name="Result2" xfId="4"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="24"/>
+    <cellStyle name="Normal 10" xfId="9" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Normal 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Normal 3" xfId="11" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Normal 4" xfId="12" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Normal 4 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="Normal 5" xfId="14" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="Normal 6" xfId="15" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="Normal 7" xfId="16" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="Normal 8" xfId="17" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="Normal 9" xfId="5" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal 9 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normale_B2020" xfId="19" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Percent 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Percent 3" xfId="22" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Percent 4" xfId="23" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Percent 5" xfId="20" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Result" xfId="3" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Result2" xfId="4" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Standard_Sce_D_Extraction" xfId="24" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -670,14 +666,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="17.125" customWidth="1"/>
     <col min="2" max="2" width="10.75" customWidth="1"/>
@@ -686,7 +682,7 @@
     <col min="19" max="19" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="14.25">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -694,7 +690,7 @@
         <v>8760</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="14.25">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -759,7 +755,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="14.25">
+    <row r="4" spans="1:18">
       <c r="A4">
         <v>2011</v>
       </c>
@@ -813,7 +809,7 @@
         <v>882798.01000000013</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="14.25">
+    <row r="5" spans="1:18">
       <c r="A5">
         <v>2012</v>
       </c>
@@ -867,7 +863,7 @@
         <v>801932.83000000019</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="14.25">
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>2013</v>
       </c>
@@ -921,7 +917,7 @@
         <v>822470.36300000013</v>
       </c>
     </row>
-    <row r="7" spans="1:18" ht="14.25">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>2014</v>
       </c>
@@ -975,7 +971,7 @@
         <v>788705.53100000008</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="14.25">
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>2015</v>
       </c>
@@ -1032,7 +1028,7 @@
         <v>754204.47399999946</v>
       </c>
     </row>
-    <row r="9" spans="1:18" ht="14.25">
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>2016</v>
       </c>
@@ -1232,187 +1228,278 @@
     <row r="16" spans="1:18" ht="15">
       <c r="A16" s="2"/>
     </row>
-    <row r="17" spans="1:12" ht="15">
-      <c r="A17" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3"/>
+    <row r="17" spans="1:13" ht="15">
+      <c r="A17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="I17" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12" ht="14.25">
-      <c r="B18" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>30</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
+      <c r="A18">
+        <v>2011</v>
+      </c>
+      <c r="B18" s="7">
+        <f>B4/$B$1</f>
+        <v>8.4906595890410959</v>
+      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
+      <c r="E18" s="3">
+        <f>E4/$B$1</f>
+        <v>23.346347602739726</v>
+      </c>
+      <c r="F18" s="7">
+        <f>F4/$B$1</f>
+        <v>12.230010273972603</v>
+      </c>
+      <c r="G18" s="3">
+        <f>G4/$B$1</f>
+        <v>44.779799315068495</v>
+      </c>
       <c r="H18" s="3"/>
       <c r="I18">
-        <v>101761.003</v>
-      </c>
-      <c r="J18">
-        <f>I18/$B$1</f>
+        <f>I4/$B$1</f>
         <v>11.616552853881279</v>
       </c>
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="1:12" ht="14.25">
-      <c r="A19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B19" s="3"/>
-      <c r="C19">
-        <v>321.39</v>
+      <c r="K18">
+        <f>K4/$B$1</f>
+        <v>2.0506392694063926E-2</v>
+      </c>
+      <c r="L18" s="3">
+        <f>L4/$B$1</f>
+        <v>4.6557077625570776E-3</v>
+      </c>
+      <c r="M18">
+        <f>M4/$B$1</f>
+        <v>0.28749680365296804</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
+      <c r="A19">
+        <v>2012</v>
+      </c>
+      <c r="B19" s="7">
+        <f t="shared" ref="B19:B23" si="4">B5/$B$1</f>
+        <v>7.6894962328767118</v>
       </c>
       <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3"/>
+      <c r="E19" s="3">
+        <f t="shared" ref="E19:G23" si="5">E5/$B$1</f>
+        <v>24.487900114155252</v>
+      </c>
+      <c r="F19" s="7">
+        <f t="shared" si="5"/>
+        <v>12.115855022831051</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" si="5"/>
+        <v>45.122265068493149</v>
+      </c>
       <c r="H19" s="3"/>
       <c r="I19">
-        <v>15939.413</v>
-      </c>
-      <c r="J19">
-        <f t="shared" ref="J19:J27" si="4">I19/$B$1</f>
+        <f t="shared" ref="I19:I23" si="6">I5/$B$1</f>
         <v>1.8195676940639269</v>
       </c>
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="1:12" ht="14.25">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="3">
-        <v>60</v>
-      </c>
-      <c r="C20" s="3">
-        <v>119.25</v>
-      </c>
+      <c r="K19">
+        <f t="shared" ref="K19:M23" si="7">K5/$B$1</f>
+        <v>1.9074543378995432E-2</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="7"/>
+        <v>9.8152968036529682E-3</v>
+      </c>
+      <c r="M19">
+        <f t="shared" si="7"/>
+        <v>0.28086963470319637</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
+      <c r="A20">
+        <v>2013</v>
+      </c>
+      <c r="B20" s="7">
+        <f t="shared" si="4"/>
+        <v>7.8269200913242019</v>
+      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
+      <c r="E20" s="3">
+        <f t="shared" si="5"/>
+        <v>26.7710051369863</v>
+      </c>
+      <c r="F20" s="7">
+        <f t="shared" si="5"/>
+        <v>12.344165525114155</v>
+      </c>
+      <c r="G20" s="3">
+        <f t="shared" si="5"/>
+        <v>45.578886073059365</v>
+      </c>
       <c r="H20" s="3"/>
       <c r="I20">
-        <v>9302.75</v>
-      </c>
-      <c r="J20">
+        <f t="shared" si="6"/>
+        <v>1.0619577625570775</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="7"/>
+        <v>1.8569863013698631E-2</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="7"/>
+        <v>9.7680365296803646E-3</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="7"/>
+        <v>0.27803835616438355</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21">
+        <v>2014</v>
+      </c>
+      <c r="B21" s="7">
         <f t="shared" si="4"/>
-        <v>1.0619577625570775</v>
-      </c>
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="1:12" ht="14.25">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="3"/>
+        <v>8.019942123287672</v>
+      </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="3">
-        <v>43400</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>32</v>
+        <f t="shared" si="5"/>
+        <v>26.417928652968037</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="5"/>
+        <v>8.2843456621004563</v>
       </c>
       <c r="G21" s="3">
-        <f>E21/110.101</f>
-        <v>394.18352240215802</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>28</v>
-      </c>
+        <f t="shared" si="5"/>
+        <v>47.02245205479452</v>
+      </c>
+      <c r="H21" s="3"/>
       <c r="I21">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J21">
+      <c r="K21">
+        <f t="shared" si="7"/>
+        <v>3.9210045662100455E-3</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="7"/>
+        <v>1.0153082191780823E-2</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="7"/>
+        <v>0.27613538812785388</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
+      <c r="A22">
+        <v>2015</v>
+      </c>
+      <c r="B22" s="7">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="1:12" ht="14.25">
-      <c r="A22" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="3">
-        <v>101</v>
-      </c>
-      <c r="C22" s="3">
-        <v>143.07</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
+        <v>8.5388726027397261</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3">
+        <f t="shared" si="5"/>
+        <v>26.554570319634703</v>
+      </c>
+      <c r="F22" s="7">
+        <f t="shared" si="5"/>
+        <v>6.5859848173515978</v>
+      </c>
+      <c r="G22" s="3">
+        <f t="shared" si="5"/>
+        <v>43.754895547945203</v>
+      </c>
       <c r="H22" s="3"/>
       <c r="I22">
-        <v>9437.2849999999999</v>
-      </c>
-      <c r="J22">
+        <f t="shared" si="6"/>
+        <v>1.0773156392694063</v>
+      </c>
+      <c r="K22">
+        <f t="shared" si="7"/>
+        <v>7.6672374429223753E-3</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="7"/>
+        <v>1.1248287671232876E-2</v>
+      </c>
+      <c r="M22">
+        <f t="shared" si="7"/>
+        <v>0.27215787671232877</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
+      <c r="A23">
+        <v>2016</v>
+      </c>
+      <c r="B23" s="7">
         <f t="shared" si="4"/>
-        <v>1.0773156392694063</v>
-      </c>
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="1:12" ht="14.25">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" s="3">
-        <v>136</v>
-      </c>
-      <c r="C23" s="3">
-        <v>112.5</v>
-      </c>
+        <v>9.3458943103881289</v>
+      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
+      <c r="E23" s="3">
+        <f t="shared" si="5"/>
+        <v>33.086409980936068</v>
+      </c>
+      <c r="F23" s="7">
+        <f t="shared" si="5"/>
+        <v>5.1864104394977169</v>
+      </c>
+      <c r="G23" s="3">
+        <f t="shared" si="5"/>
+        <v>46.599506514041096</v>
+      </c>
       <c r="H23" s="3"/>
       <c r="I23">
-        <v>17300.237000000001</v>
-      </c>
-      <c r="J23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>1.9749128995433791</v>
       </c>
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="1:12" ht="14.25">
-      <c r="A24" t="s">
-        <v>13</v>
-      </c>
-      <c r="B24" s="3">
-        <v>62</v>
-      </c>
-      <c r="C24" s="3">
-        <v>223.38</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>34</v>
-      </c>
+      <c r="K23">
+        <f t="shared" si="7"/>
+        <v>0.57075633561643835</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="7"/>
+        <v>0.74446428757442118</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="7"/>
+        <v>0.24639420913242008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -1420,19 +1507,10 @@
       <c r="I24" s="3"/>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" ht="14.25">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="3">
-        <v>195</v>
-      </c>
-      <c r="C25" s="3">
-        <v>290.33</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>35</v>
-      </c>
+    <row r="25" spans="1:13">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
@@ -1440,13 +1518,8 @@
       <c r="I25" s="3"/>
       <c r="L25" s="3"/>
     </row>
-    <row r="26" spans="1:12" ht="14.25">
-      <c r="A26" t="s">
-        <v>15</v>
-      </c>
-      <c r="B26" s="3">
-        <v>117</v>
-      </c>
+    <row r="26" spans="1:13">
+      <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -1456,10 +1529,7 @@
       <c r="I26" s="3"/>
       <c r="L26" s="3"/>
     </row>
-    <row r="27" spans="1:12" ht="14.25">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
+    <row r="27" spans="1:13">
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
@@ -1470,7 +1540,7 @@
       <c r="I27" s="3"/>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" ht="14.25">
+    <row r="28" spans="1:13">
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -1481,7 +1551,7 @@
       <c r="I28" s="3"/>
       <c r="L28" s="3"/>
     </row>
-    <row r="29" spans="1:12" ht="14.25">
+    <row r="29" spans="1:13">
       <c r="A29" t="s">
         <v>37</v>
       </c>
@@ -1492,21 +1562,21 @@
       <c r="F29" s="3"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:12" ht="14.25">
+    <row r="30" spans="1:13">
       <c r="B30" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="14.25">
+    <row r="31" spans="1:13">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:12" ht="14.25">
+    <row r="32" spans="1:13">
       <c r="B32" s="3"/>
     </row>
-    <row r="33" spans="2:2" ht="14.25">
+    <row r="33" spans="2:2">
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="2:2" ht="14.25">
+    <row r="34" spans="2:2">
       <c r="B34" s="3"/>
     </row>
   </sheetData>
@@ -1520,18 +1590,359 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC4C9AEA-3BFB-45A1-BC1F-35CEEB8F5268}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15">
+      <c r="A1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="C3">
+        <v>321.39</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3">
+        <v>60</v>
+      </c>
+      <c r="C4" s="3">
+        <v>119.25</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3">
+        <v>43400</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="3">
+        <f>E5/110.101</f>
+        <v>394.18352240215802</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="3">
+        <v>101</v>
+      </c>
+      <c r="C6" s="3">
+        <v>143.07</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>136</v>
+      </c>
+      <c r="C7" s="3">
+        <v>112.5</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="3">
+        <v>62</v>
+      </c>
+      <c r="C8" s="3">
+        <v>223.38</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="3">
+        <v>195</v>
+      </c>
+      <c r="C9" s="3">
+        <v>290.33</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3">
+        <v>117</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="8.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>45.9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3">
+        <v>15</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4">
+        <v>91.1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>118</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>960</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>778</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>443</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.9"/>
+  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="4" width="10.75" customWidth="1"/>
     <col min="5" max="5" width="8.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1545,7 +1956,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="14.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>882798.01</v>
       </c>
@@ -1561,7 +1972,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>801932.83</v>
       </c>
@@ -1577,7 +1988,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="14.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>822470.36300000001</v>
       </c>
@@ -1593,7 +2004,7 @@
         <v>2013</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>788705.53099999996</v>
       </c>
@@ -1609,7 +2020,7 @@
         <v>2014</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>760391.75999999896</v>
       </c>
@@ -1625,7 +2036,7 @@
         <v>2015</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="14.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>856331.60103615199</v>
       </c>
@@ -1648,155 +2059,4 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.75" defaultRowHeight="13.9"/>
-  <cols>
-    <col min="1" max="1" width="8.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="14.25">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1">
-        <v>34.200000000000003</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="14.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2">
-        <v>45.9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="14.25">
-      <c r="A3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="14.25">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4">
-        <v>91.1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="14.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>118</v>
-      </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="F5" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="14.25">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6">
-        <v>66</v>
-      </c>
-      <c r="D6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="14.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
-        <v>960</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="F7" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="14.25">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8">
-        <v>778</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="14.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9">
-        <v>443</v>
-      </c>
-      <c r="D9" t="s">
-        <v>53</v>
-      </c>
-      <c r="F9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
modified rough input xlsx
</commit_message>
<xml_diff>
--- a/input1.xlsx
+++ b/input1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="STOCK" sheetId="1" state="visible" r:id="rId2"/>
@@ -194,15 +194,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0%"/>
-    <numFmt numFmtId="167" formatCode="[$$-409]#,##0.00;[RED]\-[$$-409]#,##0.00"/>
-    <numFmt numFmtId="168" formatCode="0.00E+00"/>
-    <numFmt numFmtId="169" formatCode="#,##0.00\ "/>
+    <numFmt numFmtId="165" formatCode="0.00E+00"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00\ "/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -224,44 +221,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <sz val="16"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <i val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -286,18 +245,12 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDEEBF7"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -309,7 +262,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -333,153 +286,44 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="29">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="20% - Accent5 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Comma 2" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 2" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 10" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 2" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 3" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 4" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 4 2" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 5" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 6" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 7" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 8" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 9" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normal 9 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Normale_B2020" xfId="35" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Percent 2" xfId="36" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Percent 3" xfId="37" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Percent 4" xfId="38" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Percent 5" xfId="39" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 3" xfId="40" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 4" xfId="41" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Standard_Sce_D_Extraction" xfId="42" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -502,7 +346,7 @@
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFDEEBF7"/>
+      <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -551,16 +395,17 @@
   </sheetPr>
   <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="O4" activeCellId="0" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.6"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.0744186046512"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.046511627907"/>
-    <col collapsed="false" hidden="false" max="18" min="4" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0883720930233"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.293023255814"/>
+    <col collapsed="false" hidden="false" max="18" min="4" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -580,7 +425,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -623,7 +468,7 @@
       <c r="N3" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="0" t="s">
+      <c r="O3" s="2" t="s">
         <v>17</v>
       </c>
       <c r="P3" s="0" t="s">
@@ -1142,7 +987,7 @@
       <c r="A18" s="0" t="n">
         <v>2011</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="0" t="n">
         <f aca="false">B4/$B$1</f>
         <v>8.4906595890411</v>
       </c>
@@ -1152,7 +997,7 @@
         <f aca="false">E4/$B$1</f>
         <v>23.3463476027397</v>
       </c>
-      <c r="F18" s="6" t="n">
+      <c r="F18" s="0" t="n">
         <f aca="false">F4/$B$1</f>
         <v>12.2300102739726</v>
       </c>
@@ -1182,7 +1027,7 @@
       <c r="A19" s="0" t="n">
         <v>2012</v>
       </c>
-      <c r="B19" s="6" t="n">
+      <c r="B19" s="0" t="n">
         <f aca="false">B5/$B$1</f>
         <v>7.68949623287671</v>
       </c>
@@ -1191,7 +1036,7 @@
         <f aca="false">E5/$B$1</f>
         <v>24.4879001141553</v>
       </c>
-      <c r="F19" s="6" t="n">
+      <c r="F19" s="0" t="n">
         <f aca="false">F5/$B$1</f>
         <v>12.1158550228311</v>
       </c>
@@ -1221,7 +1066,7 @@
       <c r="A20" s="0" t="n">
         <v>2013</v>
       </c>
-      <c r="B20" s="6" t="n">
+      <c r="B20" s="0" t="n">
         <f aca="false">B6/$B$1</f>
         <v>7.8269200913242</v>
       </c>
@@ -1231,7 +1076,7 @@
         <f aca="false">E6/$B$1</f>
         <v>26.7710051369863</v>
       </c>
-      <c r="F20" s="6" t="n">
+      <c r="F20" s="0" t="n">
         <f aca="false">F6/$B$1</f>
         <v>12.3441655251142</v>
       </c>
@@ -1261,7 +1106,7 @@
       <c r="A21" s="0" t="n">
         <v>2014</v>
       </c>
-      <c r="B21" s="6" t="n">
+      <c r="B21" s="0" t="n">
         <f aca="false">B7/$B$1</f>
         <v>8.01994212328767</v>
       </c>
@@ -1271,7 +1116,7 @@
         <f aca="false">E7/$B$1</f>
         <v>26.417928652968</v>
       </c>
-      <c r="F21" s="6" t="n">
+      <c r="F21" s="0" t="n">
         <f aca="false">F7/$B$1</f>
         <v>8.28434566210046</v>
       </c>
@@ -1301,7 +1146,7 @@
       <c r="A22" s="0" t="n">
         <v>2015</v>
       </c>
-      <c r="B22" s="6" t="n">
+      <c r="B22" s="0" t="n">
         <f aca="false">B8/$B$1</f>
         <v>8.53887260273973</v>
       </c>
@@ -1311,7 +1156,7 @@
         <f aca="false">E8/$B$1</f>
         <v>26.5545703196347</v>
       </c>
-      <c r="F22" s="6" t="n">
+      <c r="F22" s="0" t="n">
         <f aca="false">F8/$B$1</f>
         <v>6.5859848173516</v>
       </c>
@@ -1341,7 +1186,7 @@
       <c r="A23" s="0" t="n">
         <v>2016</v>
       </c>
-      <c r="B23" s="6" t="n">
+      <c r="B23" s="0" t="n">
         <f aca="false">B9/$B$1</f>
         <v>9.34589431038813</v>
       </c>
@@ -1351,7 +1196,7 @@
         <f aca="false">E9/$B$1</f>
         <v>33.0864099809361</v>
       </c>
-      <c r="F23" s="6" t="n">
+      <c r="F23" s="0" t="n">
         <f aca="false">F9/$B$1</f>
         <v>5.18641043949772</v>
       </c>
@@ -1472,11 +1317,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10697674418605"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1673,6 +1518,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.86046511627907"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
@@ -1827,13 +1675,14 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.0744186046512"/>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.446511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.86046511627907"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>